<commit_message>
completed O(n) time O(1) space, best approach
</commit_message>
<xml_diff>
--- a/143. Reorder List/Whiteboards/Solution.xlsx
+++ b/143. Reorder List/Whiteboards/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\143. Reorder List\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B81652-93F1-4861-9643-5FF294F223AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C464D2E1-7072-4A75-91BB-E588BDD16F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>p3</t>
   </si>
 </sst>
 </file>
@@ -437,7 +449,7 @@
   <dimension ref="D2:AV66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -470,6 +482,33 @@
       <c r="W3" s="2">
         <v>8</v>
       </c>
+      <c r="AB3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>7</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>8</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="4:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1">
@@ -607,18 +646,6 @@
       <c r="AR11" s="1">
         <v>5</v>
       </c>
-      <c r="AS11" s="1">
-        <v>6</v>
-      </c>
-      <c r="AT11" s="1">
-        <v>7</v>
-      </c>
-      <c r="AU11" s="1">
-        <v>8</v>
-      </c>
-      <c r="AV11" s="1">
-        <v>9</v>
-      </c>
     </row>
     <row r="12" spans="4:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AN12" s="1">
@@ -633,12 +660,6 @@
       <c r="AQ12" s="1">
         <v>6</v>
       </c>
-      <c r="AR12" s="1">
-        <v>5</v>
-      </c>
-      <c r="AS12" s="1">
-        <v>4</v>
-      </c>
     </row>
     <row r="13" spans="4:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M13" s="1">
@@ -775,7 +796,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="13:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AP19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR20" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M21" s="1">
         <v>1</v>
       </c>
@@ -813,7 +873,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="13:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
       <c r="M22" s="1">
         <v>1</v>
       </c>
@@ -832,8 +895,11 @@
       <c r="R22" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="13:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W23" s="1">
         <v>1</v>
       </c>
@@ -855,8 +921,31 @@
       <c r="AC23" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="13:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AP24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ24" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR24" s="1">
+        <v>3</v>
+      </c>
+      <c r="AS24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M25" s="1">
         <v>1</v>
       </c>
@@ -879,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="13:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M26" s="1">
         <v>1</v>
       </c>
@@ -901,8 +990,30 @@
       <c r="S26" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="13:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO28" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP28" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W30" s="1" t="s">
         <v>3</v>
       </c>
@@ -928,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="13:37" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W31" s="1">
         <v>1</v>
       </c>

</xml_diff>